<commit_message>
function complete quarantine person
</commit_message>
<xml_diff>
--- a/scriptDatabase/quarantined_person - Copy.xlsx
+++ b/scriptDatabase/quarantined_person - Copy.xlsx
@@ -447,8 +447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,10 +530,10 @@
         <v>16</v>
       </c>
       <c r="G2">
-        <v>12312312312</v>
+        <v>12222</v>
       </c>
       <c r="H2">
-        <v>15246</v>
+        <v>1</v>
       </c>
       <c r="I2" t="s">
         <v>17</v>
@@ -545,7 +545,7 @@
         <v>13</v>
       </c>
       <c r="M2" s="1">
-        <v>44542</v>
+        <v>44545</v>
       </c>
       <c r="N2" t="s">
         <v>19</v>

</xml_diff>